<commit_message>
Sendo extraidos os dados do Sidra sobre imóveis próprios
</commit_message>
<xml_diff>
--- a/Apache-poi/Sidra.xlsx
+++ b/Apache-poi/Sidra.xlsx
@@ -224,7 +224,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -262,7 +262,7 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="M5" t="s">
+      <c r="H5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -270,31 +270,31 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
       <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>11</v>
       </c>
-      <c r="K6" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>10</v>
-      </c>
-      <c r="S6" t="s">
-        <v>11</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="L6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -308,31 +308,31 @@
       <c r="C7">
         <v>71.25</v>
       </c>
+      <c r="D7">
+        <v>14.23</v>
+      </c>
       <c r="E7">
-        <v>14.23</v>
+        <v>32.52</v>
+      </c>
+      <c r="F7">
+        <v>15.45</v>
       </c>
       <c r="G7">
-        <v>32.52</v>
+        <v>9.05</v>
+      </c>
+      <c r="H7">
+        <v>22.23</v>
       </c>
       <c r="I7">
-        <v>15.45</v>
+        <v>6.58</v>
+      </c>
+      <c r="J7">
+        <v>10.95</v>
       </c>
       <c r="K7">
-        <v>9.05</v>
-      </c>
-      <c r="M7">
-        <v>22.23</v>
-      </c>
-      <c r="O7">
-        <v>6.58</v>
-      </c>
-      <c r="Q7">
-        <v>10.95</v>
-      </c>
-      <c r="S7">
         <v>3.19</v>
       </c>
-      <c r="U7">
+      <c r="L7">
         <v>1.52</v>
       </c>
     </row>
@@ -346,31 +346,31 @@
       <c r="C8">
         <v>56.83</v>
       </c>
+      <c r="D8">
+        <v>9.92</v>
+      </c>
       <c r="E8">
-        <v>9.92</v>
+        <v>25.61</v>
+      </c>
+      <c r="F8">
+        <v>13.21</v>
       </c>
       <c r="G8">
-        <v>25.61</v>
+        <v>8.09</v>
+      </c>
+      <c r="H8">
+        <v>32.56</v>
       </c>
       <c r="I8">
-        <v>13.21</v>
+        <v>8.58</v>
+      </c>
+      <c r="J8">
+        <v>15.50</v>
       </c>
       <c r="K8">
-        <v>8.09</v>
-      </c>
-      <c r="M8">
-        <v>32.56</v>
-      </c>
-      <c r="O8">
-        <v>8.58</v>
-      </c>
-      <c r="Q8">
-        <v>15.50</v>
-      </c>
-      <c r="S8">
         <v>5.38</v>
       </c>
-      <c r="U8">
+      <c r="L8">
         <v>3.09</v>
       </c>
     </row>
@@ -384,31 +384,31 @@
       <c r="C9">
         <v>67.94</v>
       </c>
+      <c r="D9">
+        <v>13.60</v>
+      </c>
       <c r="E9">
-        <v>13.60</v>
+        <v>31.45</v>
+      </c>
+      <c r="F9">
+        <v>14.77</v>
       </c>
       <c r="G9">
-        <v>31.45</v>
+        <v>8.12</v>
+      </c>
+      <c r="H9">
+        <v>26.65</v>
       </c>
       <c r="I9">
-        <v>14.77</v>
+        <v>7.95</v>
+      </c>
+      <c r="J9">
+        <v>13.48</v>
       </c>
       <c r="K9">
-        <v>8.12</v>
-      </c>
-      <c r="M9">
-        <v>26.65</v>
-      </c>
-      <c r="O9">
-        <v>7.95</v>
-      </c>
-      <c r="Q9">
-        <v>13.48</v>
-      </c>
-      <c r="S9">
         <v>3.64</v>
       </c>
-      <c r="U9">
+      <c r="L9">
         <v>1.58</v>
       </c>
     </row>
@@ -422,31 +422,31 @@
       <c r="C10">
         <v>61.92</v>
       </c>
+      <c r="D10">
+        <v>13.06</v>
+      </c>
       <c r="E10">
-        <v>13.06</v>
+        <v>26.23</v>
+      </c>
+      <c r="F10">
+        <v>14.55</v>
       </c>
       <c r="G10">
-        <v>26.23</v>
+        <v>8.07</v>
+      </c>
+      <c r="H10">
+        <v>29.47</v>
       </c>
       <c r="I10">
-        <v>14.55</v>
+        <v>8.80</v>
+      </c>
+      <c r="J10">
+        <v>14.41</v>
       </c>
       <c r="K10">
-        <v>8.07</v>
-      </c>
-      <c r="M10">
-        <v>29.47</v>
-      </c>
-      <c r="O10">
-        <v>8.80</v>
-      </c>
-      <c r="Q10">
-        <v>14.41</v>
-      </c>
-      <c r="S10">
         <v>4.44</v>
       </c>
-      <c r="U10">
+      <c r="L10">
         <v>1.83</v>
       </c>
     </row>
@@ -460,31 +460,31 @@
       <c r="C11">
         <v>69.12</v>
       </c>
+      <c r="D11">
+        <v>13.77</v>
+      </c>
       <c r="E11">
-        <v>13.77</v>
+        <v>28.84</v>
+      </c>
+      <c r="F11">
+        <v>15.81</v>
       </c>
       <c r="G11">
-        <v>28.84</v>
+        <v>10.71</v>
+      </c>
+      <c r="H11">
+        <v>21.85</v>
       </c>
       <c r="I11">
-        <v>15.81</v>
+        <v>5.59</v>
+      </c>
+      <c r="J11">
+        <v>10.81</v>
       </c>
       <c r="K11">
-        <v>10.71</v>
-      </c>
-      <c r="M11">
-        <v>21.85</v>
-      </c>
-      <c r="O11">
-        <v>5.59</v>
-      </c>
-      <c r="Q11">
-        <v>10.81</v>
-      </c>
-      <c r="S11">
         <v>3.71</v>
       </c>
-      <c r="U11">
+      <c r="L11">
         <v>1.73</v>
       </c>
     </row>
@@ -498,31 +498,31 @@
       <c r="C12">
         <v>68.63</v>
       </c>
+      <c r="D12">
+        <v>12.67</v>
+      </c>
       <c r="E12">
-        <v>12.67</v>
+        <v>30.90</v>
+      </c>
+      <c r="F12">
+        <v>15.74</v>
       </c>
       <c r="G12">
-        <v>30.90</v>
+        <v>9.32</v>
+      </c>
+      <c r="H12">
+        <v>23.98</v>
       </c>
       <c r="I12">
-        <v>15.74</v>
+        <v>6.75</v>
+      </c>
+      <c r="J12">
+        <v>11.57</v>
       </c>
       <c r="K12">
-        <v>9.32</v>
-      </c>
-      <c r="M12">
-        <v>23.98</v>
-      </c>
-      <c r="O12">
-        <v>6.75</v>
-      </c>
-      <c r="Q12">
-        <v>11.57</v>
-      </c>
-      <c r="S12">
         <v>3.82</v>
       </c>
-      <c r="U12">
+      <c r="L12">
         <v>1.84</v>
       </c>
     </row>
@@ -536,31 +536,31 @@
       <c r="C13">
         <v>68.53</v>
       </c>
+      <c r="D13">
+        <v>13.51</v>
+      </c>
       <c r="E13">
-        <v>13.51</v>
+        <v>29.58</v>
+      </c>
+      <c r="F13">
+        <v>16.11</v>
       </c>
       <c r="G13">
-        <v>29.58</v>
+        <v>9.33</v>
+      </c>
+      <c r="H13">
+        <v>25.74</v>
       </c>
       <c r="I13">
-        <v>16.11</v>
+        <v>7.27</v>
+      </c>
+      <c r="J13">
+        <v>12.92</v>
       </c>
       <c r="K13">
-        <v>9.33</v>
-      </c>
-      <c r="M13">
-        <v>25.74</v>
-      </c>
-      <c r="O13">
-        <v>7.27</v>
-      </c>
-      <c r="Q13">
-        <v>12.92</v>
-      </c>
-      <c r="S13">
         <v>3.85</v>
       </c>
-      <c r="U13">
+      <c r="L13">
         <v>1.70</v>
       </c>
     </row>
@@ -574,31 +574,31 @@
       <c r="C14">
         <v>67.44</v>
       </c>
+      <c r="D14">
+        <v>15.09</v>
+      </c>
       <c r="E14">
-        <v>15.09</v>
+        <v>31.31</v>
+      </c>
+      <c r="F14">
+        <v>13.55</v>
       </c>
       <c r="G14">
-        <v>31.31</v>
+        <v>7.49</v>
+      </c>
+      <c r="H14">
+        <v>26.88</v>
       </c>
       <c r="I14">
-        <v>13.55</v>
+        <v>8.15</v>
+      </c>
+      <c r="J14">
+        <v>12.87</v>
       </c>
       <c r="K14">
-        <v>7.49</v>
-      </c>
-      <c r="M14">
-        <v>26.88</v>
-      </c>
-      <c r="O14">
-        <v>8.15</v>
-      </c>
-      <c r="Q14">
-        <v>12.87</v>
-      </c>
-      <c r="S14">
         <v>3.97</v>
       </c>
-      <c r="U14">
+      <c r="L14">
         <v>1.90</v>
       </c>
     </row>
@@ -612,31 +612,31 @@
       <c r="C15">
         <v>70.82</v>
       </c>
+      <c r="D15">
+        <v>13.82</v>
+      </c>
       <c r="E15">
-        <v>13.82</v>
+        <v>33.38</v>
+      </c>
+      <c r="F15">
+        <v>15.53</v>
       </c>
       <c r="G15">
-        <v>33.38</v>
+        <v>8.09</v>
+      </c>
+      <c r="H15">
+        <v>23.17</v>
       </c>
       <c r="I15">
-        <v>15.53</v>
+        <v>6.07</v>
+      </c>
+      <c r="J15">
+        <v>11.41</v>
       </c>
       <c r="K15">
-        <v>8.09</v>
-      </c>
-      <c r="M15">
-        <v>23.17</v>
-      </c>
-      <c r="O15">
-        <v>6.07</v>
-      </c>
-      <c r="Q15">
-        <v>11.41</v>
-      </c>
-      <c r="S15">
         <v>3.89</v>
       </c>
-      <c r="U15">
+      <c r="L15">
         <v>1.80</v>
       </c>
     </row>
@@ -650,31 +650,31 @@
       <c r="C16">
         <v>68.11</v>
       </c>
+      <c r="D16">
+        <v>17.20</v>
+      </c>
       <c r="E16">
-        <v>17.20</v>
+        <v>30.62</v>
+      </c>
+      <c r="F16">
+        <v>13.97</v>
       </c>
       <c r="G16">
-        <v>30.62</v>
+        <v>6.32</v>
+      </c>
+      <c r="H16">
+        <v>27.66</v>
       </c>
       <c r="I16">
-        <v>13.97</v>
+        <v>8.23</v>
+      </c>
+      <c r="J16">
+        <v>12.74</v>
       </c>
       <c r="K16">
-        <v>6.32</v>
-      </c>
-      <c r="M16">
-        <v>27.66</v>
-      </c>
-      <c r="O16">
-        <v>8.23</v>
-      </c>
-      <c r="Q16">
-        <v>12.74</v>
-      </c>
-      <c r="S16">
         <v>4.46</v>
       </c>
-      <c r="U16">
+      <c r="L16">
         <v>2.24</v>
       </c>
     </row>
@@ -688,31 +688,31 @@
       <c r="C17">
         <v>69.29</v>
       </c>
+      <c r="D17">
+        <v>13.57</v>
+      </c>
       <c r="E17">
-        <v>13.57</v>
+        <v>31.48</v>
+      </c>
+      <c r="F17">
+        <v>15.74</v>
       </c>
       <c r="G17">
-        <v>31.48</v>
+        <v>8.49</v>
+      </c>
+      <c r="H17">
+        <v>23.51</v>
       </c>
       <c r="I17">
-        <v>15.74</v>
+        <v>6.42</v>
+      </c>
+      <c r="J17">
+        <v>11.89</v>
       </c>
       <c r="K17">
-        <v>8.49</v>
-      </c>
-      <c r="M17">
-        <v>23.51</v>
-      </c>
-      <c r="O17">
-        <v>6.42</v>
-      </c>
-      <c r="Q17">
-        <v>11.89</v>
-      </c>
-      <c r="S17">
         <v>3.71</v>
       </c>
-      <c r="U17">
+      <c r="L17">
         <v>1.49</v>
       </c>
     </row>
@@ -726,31 +726,31 @@
       <c r="C18">
         <v>64.92</v>
       </c>
+      <c r="D18">
+        <v>12.75</v>
+      </c>
       <c r="E18">
-        <v>12.75</v>
+        <v>30.16</v>
+      </c>
+      <c r="F18">
+        <v>14.59</v>
       </c>
       <c r="G18">
-        <v>30.16</v>
+        <v>7.42</v>
+      </c>
+      <c r="H18">
+        <v>30.42</v>
       </c>
       <c r="I18">
-        <v>14.59</v>
+        <v>7.34</v>
+      </c>
+      <c r="J18">
+        <v>13.98</v>
       </c>
       <c r="K18">
-        <v>7.42</v>
-      </c>
-      <c r="M18">
-        <v>30.42</v>
-      </c>
-      <c r="O18">
-        <v>7.34</v>
-      </c>
-      <c r="Q18">
-        <v>13.98</v>
-      </c>
-      <c r="S18">
         <v>5.85</v>
       </c>
-      <c r="U18">
+      <c r="L18">
         <v>3.25</v>
       </c>
     </row>
@@ -764,31 +764,31 @@
       <c r="C19">
         <v>66.38</v>
       </c>
+      <c r="D19">
+        <v>11.24</v>
+      </c>
       <c r="E19">
-        <v>11.24</v>
+        <v>30.52</v>
+      </c>
+      <c r="F19">
+        <v>15.30</v>
       </c>
       <c r="G19">
-        <v>30.52</v>
+        <v>9.33</v>
+      </c>
+      <c r="H19">
+        <v>27.84</v>
       </c>
       <c r="I19">
-        <v>15.30</v>
+        <v>7.37</v>
+      </c>
+      <c r="J19">
+        <v>14.11</v>
       </c>
       <c r="K19">
-        <v>9.33</v>
-      </c>
-      <c r="M19">
-        <v>27.84</v>
-      </c>
-      <c r="O19">
-        <v>7.37</v>
-      </c>
-      <c r="Q19">
-        <v>14.11</v>
-      </c>
-      <c r="S19">
         <v>4.31</v>
       </c>
-      <c r="U19">
+      <c r="L19">
         <v>2.05</v>
       </c>
     </row>
@@ -802,31 +802,31 @@
       <c r="C20">
         <v>65.80</v>
       </c>
+      <c r="D20">
+        <v>14.74</v>
+      </c>
       <c r="E20">
-        <v>14.74</v>
+        <v>28.84</v>
+      </c>
+      <c r="F20">
+        <v>14.08</v>
       </c>
       <c r="G20">
-        <v>28.84</v>
+        <v>8.13</v>
+      </c>
+      <c r="H20">
+        <v>28.37</v>
       </c>
       <c r="I20">
-        <v>14.08</v>
+        <v>8.70</v>
+      </c>
+      <c r="J20">
+        <v>13.51</v>
       </c>
       <c r="K20">
-        <v>8.13</v>
-      </c>
-      <c r="M20">
-        <v>28.37</v>
-      </c>
-      <c r="O20">
-        <v>8.70</v>
-      </c>
-      <c r="Q20">
-        <v>13.51</v>
-      </c>
-      <c r="S20">
         <v>4.09</v>
       </c>
-      <c r="U20">
+      <c r="L20">
         <v>2.07</v>
       </c>
     </row>
@@ -840,31 +840,31 @@
       <c r="C21">
         <v>67.50</v>
       </c>
+      <c r="D21">
+        <v>15.55</v>
+      </c>
       <c r="E21">
-        <v>15.55</v>
+        <v>28.07</v>
+      </c>
+      <c r="F21">
+        <v>14.60</v>
       </c>
       <c r="G21">
-        <v>28.07</v>
+        <v>9.28</v>
+      </c>
+      <c r="H21">
+        <v>26.81</v>
       </c>
       <c r="I21">
-        <v>14.60</v>
+        <v>9.01</v>
+      </c>
+      <c r="J21">
+        <v>11.85</v>
       </c>
       <c r="K21">
-        <v>9.28</v>
-      </c>
-      <c r="M21">
-        <v>26.81</v>
-      </c>
-      <c r="O21">
-        <v>9.01</v>
-      </c>
-      <c r="Q21">
-        <v>11.85</v>
-      </c>
-      <c r="S21">
         <v>3.87</v>
       </c>
-      <c r="U21">
+      <c r="L21">
         <v>2.08</v>
       </c>
     </row>
@@ -874,26 +874,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A1:V1"/>
-    <mergeCell ref="A2:V2"/>
+  <mergeCells count="9">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:V3"/>
-    <mergeCell ref="C4:V4"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="M5:V5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="A22:V22"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="A22:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dados sendo inseridos no banco
</commit_message>
<xml_diff>
--- a/Apache-poi/Sidra.xlsx
+++ b/Apache-poi/Sidra.xlsx
@@ -1,21 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Documents\2° Semestre ADS\ProjetoAPdata\Apache-poi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0E547A-7712-4CC3-8D6D-DC3EBAF7C368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="48" windowWidth="13332" windowHeight="4200" activeTab="0"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabela" sheetId="1" r:id="rId3"/>
-    <sheet name="Notas" sheetId="2" r:id="rId4"/>
+    <sheet name="Tabela" sheetId="1" r:id="rId1"/>
+    <sheet name="Notas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Tabela 9929 - Domicílios particulares permanentes ocupados, por condição de ocupação do domicílio, segundo o número de moradores com 15 anos ou mais de idade e número de moradores com 14 anos ou menos de idade</t>
   </si>
@@ -57,48 +76,6 @@
   </si>
   <si>
     <t>Brasil</t>
-  </si>
-  <si>
-    <t>Barueri (SP)</t>
-  </si>
-  <si>
-    <t>Campinas (SP)</t>
-  </si>
-  <si>
-    <t>Diadema (SP)</t>
-  </si>
-  <si>
-    <t>Guarujá (SP)</t>
-  </si>
-  <si>
-    <t>Guarulhos (SP)</t>
-  </si>
-  <si>
-    <t>Osasco (SP)</t>
-  </si>
-  <si>
-    <t>Praia Grande (SP)</t>
-  </si>
-  <si>
-    <t>Santo André (SP)</t>
-  </si>
-  <si>
-    <t>Santos (SP)</t>
-  </si>
-  <si>
-    <t>São Bernardo do Campo (SP)</t>
-  </si>
-  <si>
-    <t>São Caetano do Sul (SP)</t>
-  </si>
-  <si>
-    <t>São José dos Campos (SP)</t>
-  </si>
-  <si>
-    <t>São Paulo (SP)</t>
-  </si>
-  <si>
-    <t>São Vicente (SP)</t>
   </si>
   <si>
     <t>Fonte: IBGE - Censo Demográfico</t>
@@ -161,19 +138,61 @@
   <si>
     <t>Significa uma faixa de valores. Varia em função da tabela (se for o caso).
 Ex: O nível de precisão da produção estimada de combustíveis está na faixa A (95 a 100%)</t>
+  </si>
+  <si>
+    <t>São Vicente</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
+  </si>
+  <si>
+    <t>São José dos Campos</t>
+  </si>
+  <si>
+    <t>São Caetano do Sul</t>
+  </si>
+  <si>
+    <t>São Bernardo do Campo</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Santo André</t>
+  </si>
+  <si>
+    <t>Praia Grande</t>
+  </si>
+  <si>
+    <t>Osasco</t>
+  </si>
+  <si>
+    <t>Guarulhos</t>
+  </si>
+  <si>
+    <t>Guarujá</t>
+  </si>
+  <si>
+    <t>Diadema</t>
+  </si>
+  <si>
+    <t>Campinas</t>
+  </si>
+  <si>
+    <t>Barueri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <color indexed="64"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,7 +203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -192,26 +211,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -219,54 +224,404 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+  <a:themeElements>
+    <a:clrScheme name="Office 2007 - 2010">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office 2007 - 2010">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office 2007 - 2010">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="C4" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -298,7 +653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -312,13 +667,13 @@
         <v>14.23</v>
       </c>
       <c r="E7">
-        <v>32.52</v>
+        <v>32.520000000000003</v>
       </c>
       <c r="F7">
         <v>15.45</v>
       </c>
       <c r="G7">
-        <v>9.05</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="H7">
         <v>22.23</v>
@@ -336,9 +691,9 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -365,7 +720,7 @@
         <v>8.58</v>
       </c>
       <c r="J8">
-        <v>15.50</v>
+        <v>15.5</v>
       </c>
       <c r="K8">
         <v>5.38</v>
@@ -374,9 +729,9 @@
         <v>3.09</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -385,7 +740,7 @@
         <v>67.94</v>
       </c>
       <c r="D9">
-        <v>13.60</v>
+        <v>13.6</v>
       </c>
       <c r="E9">
         <v>31.45</v>
@@ -394,7 +749,7 @@
         <v>14.77</v>
       </c>
       <c r="G9">
-        <v>8.12</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="H9">
         <v>26.65</v>
@@ -412,9 +767,9 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -438,21 +793,21 @@
         <v>29.47</v>
       </c>
       <c r="I10">
-        <v>8.80</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="J10">
         <v>14.41</v>
       </c>
       <c r="K10">
-        <v>4.44</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="L10">
         <v>1.83</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -488,9 +843,9 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -502,7 +857,7 @@
         <v>12.67</v>
       </c>
       <c r="E12">
-        <v>30.90</v>
+        <v>30.9</v>
       </c>
       <c r="F12">
         <v>15.74</v>
@@ -526,9 +881,9 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -561,12 +916,12 @@
         <v>3.85</v>
       </c>
       <c r="L13">
-        <v>1.70</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -599,24 +954,24 @@
         <v>3.97</v>
       </c>
       <c r="L14">
-        <v>1.90</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15">
-        <v>70.82</v>
+        <v>70.819999999999993</v>
       </c>
       <c r="D15">
         <v>13.82</v>
       </c>
       <c r="E15">
-        <v>33.38</v>
+        <v>33.380000000000003</v>
       </c>
       <c r="F15">
         <v>15.53</v>
@@ -637,12 +992,12 @@
         <v>3.89</v>
       </c>
       <c r="L15">
-        <v>1.80</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -651,7 +1006,7 @@
         <v>68.11</v>
       </c>
       <c r="D16">
-        <v>17.20</v>
+        <v>17.2</v>
       </c>
       <c r="E16">
         <v>30.62</v>
@@ -675,18 +1030,18 @@
         <v>4.46</v>
       </c>
       <c r="L16">
-        <v>2.24</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17">
-        <v>69.29</v>
+        <v>69.290000000000006</v>
       </c>
       <c r="D17">
         <v>13.57</v>
@@ -716,9 +1071,9 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -754,9 +1109,9 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -771,7 +1126,7 @@
         <v>30.52</v>
       </c>
       <c r="F19">
-        <v>15.30</v>
+        <v>15.3</v>
       </c>
       <c r="G19">
         <v>9.33</v>
@@ -786,21 +1141,21 @@
         <v>14.11</v>
       </c>
       <c r="K19">
-        <v>4.31</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="L19">
-        <v>2.05</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
       <c r="C20">
-        <v>65.80</v>
+        <v>65.8</v>
       </c>
       <c r="D20">
         <v>14.74</v>
@@ -812,13 +1167,13 @@
         <v>14.08</v>
       </c>
       <c r="G20">
-        <v>8.13</v>
+        <v>8.1300000000000008</v>
       </c>
       <c r="H20">
         <v>28.37</v>
       </c>
       <c r="I20">
-        <v>8.70</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J20">
         <v>13.51</v>
@@ -827,18 +1182,18 @@
         <v>4.09</v>
       </c>
       <c r="L20">
-        <v>2.07</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21">
-        <v>67.50</v>
+        <v>67.5</v>
       </c>
       <c r="D21">
         <v>15.55</v>
@@ -847,10 +1202,10 @@
         <v>28.07</v>
       </c>
       <c r="F21">
-        <v>14.60</v>
+        <v>14.6</v>
       </c>
       <c r="G21">
-        <v>9.28</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="H21">
         <v>26.81</v>
@@ -868,13 +1223,25 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A22:L22"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A3:A6"/>
@@ -883,96 +1250,95 @@
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="H5:L5"/>
-    <mergeCell ref="A22:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="B11" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>